<commit_message>
Update new DB HaiPM
</commit_message>
<xml_diff>
--- a/ projectquanlybongdavodichquocgia/Document/Bao Cao Lan2/CSDL Moi.xlsx
+++ b/ projectquanlybongdavodichquocgia/Document/Bao Cao Lan2/CSDL Moi.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1075" uniqueCount="692">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1079" uniqueCount="696">
   <si>
     <t>BHL</t>
   </si>
@@ -2095,19 +2095,38 @@
   </si>
   <si>
     <t xml:space="preserve">select row_number() over (order by tongdiem desc,sobanghiduoc desc,sobanbilotluoi asc) as 'Ha_x001E_ng',  MaDB, TenDB, tongdiem ongdie_x001E_m', sobanghiduoc 'obanghiduoc', sobanbilotluoi 'Sobanbilotluoi' from DoiBong db </t>
+  </si>
+  <si>
+    <t>THAMSO</t>
+  </si>
+  <si>
+    <t>MATHAMSO(NVARCHAR(10))</t>
+  </si>
+  <si>
+    <t>GIATRI(NVARCHAR(100))</t>
+  </si>
+  <si>
+    <t>TENTHAMSO(NVARCHAR(20))</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="5">
+  <fonts count="6">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="128"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -2164,12 +2183,13 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2473,8 +2493,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AZ26"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="Q21" sqref="Q21"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="AG23" sqref="AG23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="2.42578125" defaultRowHeight="15"/>
@@ -2713,20 +2733,32 @@
       <c r="A23" s="3" t="s">
         <v>52</v>
       </c>
+      <c r="N23" s="3" t="s">
+        <v>692</v>
+      </c>
     </row>
     <row r="24" spans="1:52">
       <c r="B24" s="1" t="s">
         <v>17</v>
       </c>
+      <c r="N24" s="1" t="s">
+        <v>693</v>
+      </c>
     </row>
     <row r="25" spans="1:52">
       <c r="B25" t="s">
         <v>53</v>
       </c>
+      <c r="N25" s="5" t="s">
+        <v>695</v>
+      </c>
     </row>
     <row r="26" spans="1:52">
       <c r="B26" t="s">
         <v>9</v>
+      </c>
+      <c r="N26" s="5" t="s">
+        <v>694</v>
       </c>
     </row>
   </sheetData>

</xml_diff>